<commit_message>
test excel selection and drop droplist menus
</commit_message>
<xml_diff>
--- a/tabla comparativa.xlsx
+++ b/tabla comparativa.xlsx
@@ -513,50 +513,50 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jonás Ramalho</t>
+          <t>Jared Olmos</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6.98</v>
+        <v>4.6</v>
       </c>
       <c r="C2" t="n">
-        <v>4.07</v>
+        <v>5.89</v>
       </c>
       <c r="D2" t="n">
-        <v>51.43</v>
+        <v>40.8</v>
       </c>
       <c r="E2" t="n">
-        <v>2.09</v>
+        <v>3.1</v>
       </c>
       <c r="F2" t="n">
-        <v>44.44</v>
+        <v>40.53</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>4.88</v>
+        <v>3.44</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>36.86</v>
+        <v>23.5</v>
       </c>
       <c r="K2" t="n">
-        <v>86.75</v>
+        <v>74.3</v>
       </c>
       <c r="L2" t="n">
-        <v>13.26</v>
+        <v>12.45</v>
       </c>
       <c r="M2" t="n">
-        <v>75.44</v>
+        <v>60.78</v>
       </c>
       <c r="N2" t="n">
-        <v>4.65</v>
+        <v>5.7</v>
       </c>
       <c r="O2" t="n">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">

</xml_diff>